<commit_message>
Fix translation issue on data editor entry
</commit_message>
<xml_diff>
--- a/data/service_es.xlsx
+++ b/data/service_es.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Data Editor</t>
   </si>
   <si>
-    <t xml:space="preserve">Since 2025</t>
+    <t xml:space="preserve">Desde 2025</t>
   </si>
   <si>
     <t xml:space="preserve">\href{https://royalsocietypublishing.org/journal/rspb}{Proceedings of the Royal Society B}</t>
@@ -499,10 +499,10 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4296875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.29"/>
@@ -529,7 +529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -546,7 +546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -564,7 +564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -586,7 +586,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -608,7 +608,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -630,7 +630,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -743,12 +743,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E28" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>51</v>
       </c>

</xml_diff>